<commit_message>
added qn num, adjusted qn space
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djgvk\PycharmProjects\testQuiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23ECC66-7C76-4730-9750-F0D0AB95AE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715B1B81-195B-4327-B487-A85FE9BD226D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quiz" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="114">
   <si>
     <t>Multiple Choice</t>
   </si>
@@ -130,9 +130,6 @@
     <t>like fractions</t>
   </si>
   <si>
-    <t>In a garden there are 5 flowers and 2 of them are yellow in color. How to mention this in mathematics?</t>
-  </si>
-  <si>
     <t>2/5</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>not all</t>
   </si>
   <si>
-    <t>There are 3 group of baloons. In each group 3 baloons are there. Out of which 7 were bursted. How will you represent this in fraction?</t>
-  </si>
-  <si>
     <t>6/3</t>
   </si>
   <si>
@@ -209,6 +203,179 @@
   </si>
   <si>
     <t>whole number+proper fraction - this combination is called:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 7 rotis. Out of them, 2 rotis were eaten by Kabila. 1 was eaten by Guru. 
+1. What part of rotis Kabila eat?
+</t>
+  </si>
+  <si>
+    <t>1/7</t>
+  </si>
+  <si>
+    <t>3/7</t>
+  </si>
+  <si>
+    <t>4/7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 7 rotis. Out of them, 2 rotis were eaten by Kabila. 1 was eaten by Guru. 
+1. What part of rotis Guru ate?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are 7 rotis. Out of them, 2 rotis were eaten by Kabila. 1 was eaten by Guru. 
+1. What part of rotis left?
+</t>
+  </si>
+  <si>
+    <t>4/10</t>
+  </si>
+  <si>
+    <t>3 4/10</t>
+  </si>
+  <si>
+    <t>34/10</t>
+  </si>
+  <si>
+    <t>How a mixed fraction looks like?</t>
+  </si>
+  <si>
+    <t>whole num . Nr/Dr</t>
+  </si>
+  <si>
+    <t>whole num . Dr/Nr</t>
+  </si>
+  <si>
+    <t>Nr/Dr . Whole num</t>
+  </si>
+  <si>
+    <t>whole num</t>
+  </si>
+  <si>
+    <t>If a fraction has 1 in the Numerator</t>
+  </si>
+  <si>
+    <t>like fraction</t>
+  </si>
+  <si>
+    <t>In a group of 7 baloons, 1 baloon is red. How you say this in fraction?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>none of the above</t>
+  </si>
+  <si>
+    <t>Nr is 1</t>
+  </si>
+  <si>
+    <t>Dr is 1</t>
+  </si>
+  <si>
+    <t>what are a like fractions?</t>
+  </si>
+  <si>
+    <t>Nr of the fractions are same</t>
+  </si>
+  <si>
+    <t>Dr of the fractions are the same</t>
+  </si>
+  <si>
+    <t>The concept of the like fractions - have minimum how many fractions are needed?</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Raju has 7 sweets and Ramesh has 7 sweets. Raju ate all the sweets but Ramesh ate 4 sweets. 
+Fraction of sweets Raju ate = ?
+Fraction of sweets Ramesh ate = ?</t>
+  </si>
+  <si>
+    <t>7/7,  4/7</t>
+  </si>
+  <si>
+    <t>4/7,  7/7</t>
+  </si>
+  <si>
+    <t>5/7,  4/7</t>
+  </si>
+  <si>
+    <t>4/7,  3/7</t>
+  </si>
+  <si>
+    <t>1/7, 2/7, 3/7, 4/5,  6/2, 1/3,  4/7,  4/7 -what are the like fractions in these given fractions?</t>
+  </si>
+  <si>
+    <t>1/7,  2/7,  3/7, 4/7</t>
+  </si>
+  <si>
+    <t>4/5, 6/2, 1/3</t>
+  </si>
+  <si>
+    <t>1/7, 2/7</t>
+  </si>
+  <si>
+    <t>1/7, 2/7, 3/7, 4/5,  6/2, 1/3,  4/7,  4/7 -what are the unlike fractions in these given fractions?</t>
+  </si>
+  <si>
+    <t>1/7,  1/3,  4/5, 6/2</t>
+  </si>
+  <si>
+    <t>By checking what information, you decide like or unlike fractions?</t>
+  </si>
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>Dr</t>
+  </si>
+  <si>
+    <t>whole number</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>Two or more fractions have same denominators - called?</t>
+  </si>
+  <si>
+    <t>unlike fractions</t>
+  </si>
+  <si>
+    <t>Two or more fractions have different denominators?</t>
+  </si>
+  <si>
+    <t>In a garden there are 5 flowers and 2 of them are yellow in color. 
+How to mention this in mathematics?</t>
+  </si>
+  <si>
+    <t>There are 3 group of baloons. In each group 3 baloons are there. 
+Out of which 7 were bursted. 
+How will you represent this in fraction?</t>
+  </si>
+  <si>
+    <t>On your birthday, your family consumed 3 cakes completely. 
+Then you cut another cake into 10 pieces and out of them, your family had 4 pieces. 
+How do you represent this in mathematics?</t>
+  </si>
+  <si>
+    <t>Out of 8 butterflies one of them was in red color. 
+So, what is the fraction of butterflies are red? Is this unit fraction?</t>
   </si>
 </sst>
 </file>
@@ -492,6 +659,139 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>516255</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1239185" cy="165366"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A063FC-7117-EA66-1033-7F7B7F98F0E1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8450580" y="2977515"/>
+              <a:ext cx="1239185" cy="165366"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <a:fld id="{825F15A7-03F4-43D7-82C5-3E23DA2F108C}" type="mathplaceholder">
+                      <a:rPr lang="en-IN" sz="1100" i="1" kern="1200">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <a:t>Type equation here.</a:t>
+                    </a:fld>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-IN" sz="1100" kern="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A063FC-7117-EA66-1033-7F7B7F98F0E1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8450580" y="2977515"/>
+              <a:ext cx="1239185" cy="165366"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100" i="0" kern="1200">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>"Type equation here."</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-IN" sz="1100" kern="1200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -692,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -901,22 +1201,22 @@
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="6">
         <v>3</v>
@@ -933,7 +1233,7 @@
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>0</v>
@@ -948,7 +1248,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="6">
         <v>3</v>
@@ -965,22 +1265,22 @@
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="G9" s="6">
         <v>1</v>
@@ -997,7 +1297,7 @@
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>0</v>
@@ -1012,7 +1312,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="6">
         <v>1</v>
@@ -1029,7 +1329,7 @@
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>0</v>
@@ -1044,7 +1344,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="6">
         <v>2</v>
@@ -1061,7 +1361,7 @@
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>0</v>
@@ -1076,7 +1376,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="6">
         <v>2</v>
@@ -1093,7 +1393,7 @@
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>0</v>
@@ -1108,7 +1408,7 @@
         <v>25</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="6">
         <v>3</v>
@@ -1125,22 +1425,22 @@
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1">
       <c r="A14" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="G14" s="6">
         <v>1</v>
@@ -1155,24 +1455,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1">
+    <row r="15" spans="1:10" ht="12.6" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="F15" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="6">
         <v>2</v>
@@ -1189,7 +1489,7 @@
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>0</v>
@@ -1219,196 +1519,553 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" ht="12.75" customHeight="1">
+    <row r="17" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>20</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="6">
+        <v>2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>20</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="6">
+        <v>4</v>
+      </c>
+      <c r="H19" s="5">
+        <v>20</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="6">
+        <v>3</v>
+      </c>
+      <c r="H20" s="5">
+        <v>20</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="6">
+        <v>3</v>
+      </c>
+      <c r="H21" s="5">
+        <v>20</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>20</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A23" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="6">
+        <v>4</v>
+      </c>
+      <c r="H23" s="5">
+        <v>20</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A24" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>20</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A25" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2</v>
+      </c>
+      <c r="H25" s="5">
+        <v>20</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A26" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4</v>
+      </c>
+      <c r="H26" s="5">
+        <v>20</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A27" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="6">
+        <v>2</v>
+      </c>
+      <c r="H27" s="5">
+        <v>20</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
+        <v>20</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A29" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>20</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A30" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="6">
+        <v>2</v>
+      </c>
+      <c r="H30" s="5">
+        <v>20</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A31" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="6">
+        <v>2</v>
+      </c>
+      <c r="H31" s="5">
+        <v>20</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="6">
+        <v>3</v>
+      </c>
+      <c r="H32" s="5">
+        <v>20</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" s="6">
+        <v>4</v>
+      </c>
+      <c r="H33" s="5">
+        <v>20</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="12.75" customHeight="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="11"/>
@@ -1417,9 +2074,9 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:9" ht="12.75" customHeight="1">
+    <row r="35" spans="1:10" ht="12.75" customHeight="1">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="11"/>
@@ -1428,9 +2085,9 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:9" ht="12.75" customHeight="1">
+    <row r="36" spans="1:10" ht="12.75" customHeight="1">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="11"/>
@@ -1439,9 +2096,9 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9" ht="12.75" customHeight="1">
+    <row r="37" spans="1:10" ht="12.75" customHeight="1">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="11"/>
@@ -1450,9 +2107,9 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9" ht="12.75" customHeight="1">
+    <row r="38" spans="1:10" ht="12.75" customHeight="1">
       <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="11"/>
@@ -1461,7 +2118,7 @@
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="1:9" ht="12.75" customHeight="1">
+    <row r="39" spans="1:10" ht="12.75" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="17"/>
@@ -1472,7 +2129,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9" ht="12.75" customHeight="1">
+    <row r="40" spans="1:10" ht="12.75" customHeight="1">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="17"/>
@@ -1483,7 +2140,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:9" ht="12.75" customHeight="1">
+    <row r="41" spans="1:10" ht="12.75" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="17"/>
@@ -1494,7 +2151,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:9" ht="12.75" customHeight="1">
+    <row r="42" spans="1:10" ht="12.75" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="17"/>
@@ -1505,7 +2162,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9" ht="12.75" customHeight="1">
+    <row r="43" spans="1:10" ht="12.75" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="17"/>
@@ -1516,7 +2173,7 @@
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1">
+    <row r="44" spans="1:10" ht="12.75" customHeight="1">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="17"/>
@@ -1527,7 +2184,7 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9" ht="12.75" customHeight="1">
+    <row r="45" spans="1:10" ht="12.75" customHeight="1">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="17"/>
@@ -1538,7 +2195,7 @@
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:9" ht="12.75" customHeight="1">
+    <row r="46" spans="1:10" ht="12.75" customHeight="1">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="17"/>
@@ -1549,7 +2206,7 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:9" ht="12.75" customHeight="1">
+    <row r="47" spans="1:10" ht="12.75" customHeight="1">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="17"/>
@@ -1560,7 +2217,7 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="1:9" ht="12.75" customHeight="1">
+    <row r="48" spans="1:10" ht="12.75" customHeight="1">
       <c r="A48" s="4"/>
       <c r="B48" s="5"/>
       <c r="C48" s="17"/>
@@ -5752,7 +6409,7 @@
       <formula>AND(OR(NOT(ISBLANK($B2)),NOT(ISBLANK($C2)),NOT(ISBLANK($D2)),NOT(ISBLANK($E2)),NOT(ISBLANK($F2)),NOT(ISBLANK(#REF!)),NOT(ISBLANK($G2)),NOT(ISBLANK($H2)),NOT(ISBLANK($I2))),ISBLANK($A2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J6 A2:H101">
+  <conditionalFormatting sqref="A2:H101 J3 J6">
     <cfRule type="notContainsBlanks" dxfId="14" priority="14">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
@@ -5827,5 +6484,6 @@
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>